<commit_message>
GUION 3 GRADO 8 DEFINITIVOS
UNICAMENTE FALTA RECURSO 170. Necesito ayuda para ubicar motor adecuado.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/EsqueletoGuion_CS_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/EsqueletoGuion_CS_08_02_CO.xlsx
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'CUADERNO DEL PROFESOR'!$C$1:$C$30</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="106">
   <si>
     <t>FICHA</t>
   </si>
@@ -160,9 +160,6 @@
     <t>Reformas administrativas y económicas</t>
   </si>
   <si>
-    <t>Practica: Los virreinatos españoles en América</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reforma eclesiástica </t>
   </si>
   <si>
@@ -229,9 +226,6 @@
     <t>La creación de Bolivia</t>
   </si>
   <si>
-    <t>Practica: Las batallas que definieron la Independencia</t>
-  </si>
-  <si>
     <t>Independencia del Río de la Plata</t>
   </si>
   <si>
@@ -241,18 +235,12 @@
     <t>Encuentra el hecho o el personaje de la Independencia</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Conoce el pensamiento de Simón Bolívar</t>
-  </si>
-  <si>
     <t>Independencia de las colonias de Centroamérica</t>
   </si>
   <si>
     <t>El Grito de Dolores, en México</t>
   </si>
   <si>
-    <t>Practica: Los principios del Plan de Iguala</t>
-  </si>
-  <si>
     <t>Independencia de El Salvador</t>
   </si>
   <si>
@@ -280,9 +268,6 @@
     <t>Refuerza tu aprendizaje: Los caudillos</t>
   </si>
   <si>
-    <t>Practica: La independencia de Centroamérica</t>
-  </si>
-  <si>
     <t>Manifestaciones artísticas y culturales</t>
   </si>
   <si>
@@ -337,13 +322,31 @@
     <t>Refuerza tu aprendizaje: La Independencia centroamericana</t>
   </si>
   <si>
-    <t>Practica: La Independencia de Centroamérica</t>
-  </si>
-  <si>
     <t>La Independencia de las colonias americanas</t>
   </si>
   <si>
-    <t>Competencias: cronología de la Independencia americana</t>
+    <t>Competencias: Cronología de la Independencia americana</t>
+  </si>
+  <si>
+    <t>Los virreinatos españoles en América</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Los virreinatos españoles en América</t>
+  </si>
+  <si>
+    <t>Simón Bolívar y la Independencia</t>
+  </si>
+  <si>
+    <t>Los principios del Plan de Iguala</t>
+  </si>
+  <si>
+    <t>Las batallas que definieron la Independencia</t>
+  </si>
+  <si>
+    <t>La Independencia de Centroamérica</t>
+  </si>
+  <si>
+    <t>La independencia de Centroamérica</t>
   </si>
 </sst>
 </file>
@@ -1876,19 +1879,19 @@
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1904,19 +1907,19 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1924,19 +1927,19 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
         <v>93</v>
-      </c>
-      <c r="C4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" t="s">
-        <v>98</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -1944,19 +1947,19 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
         <v>93</v>
-      </c>
-      <c r="C5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E5" t="s">
-        <v>98</v>
       </c>
       <c r="F5">
         <v>9</v>
@@ -1964,19 +1967,19 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
         <v>93</v>
-      </c>
-      <c r="C6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" t="s">
-        <v>98</v>
       </c>
       <c r="F6">
         <v>18</v>
@@ -1998,7 +2001,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2020,7 +2023,7 @@
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="B2" s="54" t="s">
         <v>33</v>
@@ -2032,7 +2035,7 @@
     </row>
     <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="54" t="s">
         <v>33</v>
@@ -2044,7 +2047,7 @@
     </row>
     <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="54" t="s">
         <v>33</v>
@@ -2056,7 +2059,7 @@
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="54" t="s">
         <v>33</v>
@@ -2067,7 +2070,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="54" t="s">
         <v>33</v>
@@ -2078,7 +2081,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="B7" s="54" t="s">
         <v>33</v>
@@ -2089,7 +2092,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="B8" s="54" t="s">
         <v>33</v>
@@ -2100,7 +2103,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" s="54" t="s">
         <v>33</v>
@@ -2111,7 +2114,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="B10" s="54" t="s">
         <v>33</v>
@@ -2122,7 +2125,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="B11" s="54" t="s">
         <v>33</v>
@@ -2133,7 +2136,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B12" s="54" t="s">
         <v>33</v>
@@ -2144,7 +2147,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B13" s="54" t="s">
         <v>33</v>
@@ -2155,7 +2158,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B14" s="54" t="s">
         <v>33</v>
@@ -2166,7 +2169,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B15" s="54" t="s">
         <v>33</v>
@@ -2232,7 +2235,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2270,7 +2273,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="C3" s="51" t="s">
         <v>33</v>
@@ -2282,7 +2285,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="53" t="s">
         <v>34</v>
@@ -2294,7 +2297,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="51" t="s">
         <v>33</v>
@@ -2306,7 +2309,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="53" t="s">
         <v>34</v>
@@ -2318,7 +2321,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="51" t="s">
         <v>33</v>
@@ -2330,7 +2333,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="51" t="s">
         <v>33</v>
@@ -2342,7 +2345,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="51" t="s">
         <v>33</v>
@@ -2354,7 +2357,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C10" s="53" t="s">
         <v>34</v>
@@ -2366,7 +2369,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="C11" s="51" t="s">
         <v>33</v>
@@ -2378,7 +2381,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="C12" s="51" t="s">
         <v>33</v>
@@ -2390,7 +2393,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C13" s="51" t="s">
         <v>33</v>
@@ -2402,7 +2405,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="C14" s="53" t="s">
         <v>34</v>
@@ -2414,7 +2417,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C15" s="51" t="s">
         <v>33</v>
@@ -2426,7 +2429,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C16" s="53" t="s">
         <v>34</v>
@@ -2438,7 +2441,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C17" s="51" t="s">
         <v>33</v>
@@ -2450,7 +2453,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C18" s="51" t="s">
         <v>33</v>
@@ -2462,7 +2465,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="52" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C19" s="53" t="s">
         <v>34</v>
@@ -2474,7 +2477,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C20" s="53" t="s">
         <v>33</v>
@@ -2558,8 +2561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E49" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="D76" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="H99" sqref="H99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2611,7 +2614,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>23</v>
@@ -2629,7 +2632,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>28</v>
@@ -2647,7 +2650,7 @@
         <v>39</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>24</v>
@@ -2665,7 +2668,7 @@
         <v>39</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="20" t="s">
@@ -2685,7 +2688,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="20" t="s">
@@ -2705,7 +2708,7 @@
         <v>39</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="20" t="s">
@@ -2725,7 +2728,7 @@
         <v>39</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="20" t="s">
@@ -2751,7 +2754,7 @@
         <v>39</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="20" t="s">
@@ -2773,7 +2776,7 @@
         <v>39</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="20" t="s">
@@ -2787,7 +2790,7 @@
         <v>26</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="I10" s="21" t="s">
         <v>33</v>
@@ -2801,7 +2804,7 @@
         <v>39</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="20" t="s">
@@ -2823,7 +2826,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="20" t="s">
@@ -2845,7 +2848,7 @@
         <v>39</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="20" t="s">
@@ -2853,7 +2856,7 @@
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>23</v>
@@ -2867,7 +2870,7 @@
         <v>39</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="20" t="s">
@@ -2875,7 +2878,7 @@
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>28</v>
@@ -2889,7 +2892,7 @@
         <v>39</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="20" t="s">
@@ -2897,7 +2900,7 @@
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>23</v>
@@ -2911,7 +2914,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="20" t="s">
@@ -2919,7 +2922,7 @@
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>24</v>
@@ -2933,7 +2936,7 @@
         <v>39</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="20" t="s">
@@ -2941,13 +2944,13 @@
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>34</v>
@@ -2961,7 +2964,7 @@
         <v>39</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="20" t="s">
@@ -2969,13 +2972,13 @@
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>33</v>
@@ -2989,11 +2992,11 @@
         <v>39</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>23</v>
@@ -3009,11 +3012,11 @@
         <v>39</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>23</v>
@@ -3029,11 +3032,11 @@
         <v>39</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>28</v>
@@ -3049,11 +3052,11 @@
         <v>39</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C22" s="23"/>
       <c r="D22" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>23</v>
@@ -3069,11 +3072,11 @@
         <v>39</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>28</v>
@@ -3089,11 +3092,11 @@
         <v>39</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="20" t="s">
         <v>27</v>
@@ -3101,7 +3104,7 @@
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I24" s="21" t="s">
         <v>34</v>
@@ -3115,11 +3118,11 @@
         <v>39</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>23</v>
@@ -3135,11 +3138,11 @@
         <v>39</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C26" s="23"/>
       <c r="D26" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>26</v>
@@ -3147,7 +3150,7 @@
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I26" s="21" t="s">
         <v>33</v>
@@ -3161,11 +3164,11 @@
         <v>39</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C27" s="23"/>
       <c r="D27" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>29</v>
@@ -3181,11 +3184,11 @@
         <v>39</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>24</v>
@@ -3201,7 +3204,7 @@
         <v>39</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C29" s="23"/>
       <c r="D29" s="20" t="s">
@@ -3221,7 +3224,7 @@
         <v>39</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="20" t="s">
@@ -3233,7 +3236,7 @@
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
       <c r="H30" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I30" s="21" t="s">
         <v>33</v>
@@ -3247,7 +3250,7 @@
         <v>39</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="37" t="s">
         <v>23</v>
@@ -3265,11 +3268,11 @@
         <v>39</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="37"/>
       <c r="D32" s="38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E32" s="38" t="s">
         <v>23</v>
@@ -3285,11 +3288,11 @@
         <v>39</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="37"/>
       <c r="D33" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E33" s="38" t="s">
         <v>23</v>
@@ -3305,11 +3308,11 @@
         <v>39</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="37"/>
       <c r="D34" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E34" s="38" t="s">
         <v>28</v>
@@ -3325,11 +3328,11 @@
         <v>39</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" s="37"/>
       <c r="D35" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E35" s="38" t="s">
         <v>23</v>
@@ -3345,11 +3348,11 @@
         <v>39</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" s="37"/>
       <c r="D36" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E36" s="38" t="s">
         <v>28</v>
@@ -3365,11 +3368,11 @@
         <v>39</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C37" s="37"/>
       <c r="D37" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E37" s="38" t="s">
         <v>26</v>
@@ -3377,7 +3380,7 @@
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
       <c r="H37" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I37" s="39" t="s">
         <v>33</v>
@@ -3391,11 +3394,11 @@
         <v>39</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" s="37"/>
       <c r="D38" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E38" s="38" t="s">
         <v>23</v>
@@ -3411,11 +3414,11 @@
         <v>39</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39" s="37"/>
       <c r="D39" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E39" s="38" t="s">
         <v>27</v>
@@ -3423,7 +3426,7 @@
       <c r="F39" s="38"/>
       <c r="G39" s="38"/>
       <c r="H39" s="40" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I39" s="38" t="s">
         <v>34</v>
@@ -3437,15 +3440,15 @@
         <v>39</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" s="37"/>
       <c r="D40" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E40" s="38"/>
       <c r="F40" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G40" s="38" t="s">
         <v>23</v>
@@ -3459,15 +3462,15 @@
         <v>39</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C41" s="37"/>
       <c r="D41" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E41" s="38"/>
       <c r="F41" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G41" s="38" t="s">
         <v>28</v>
@@ -3481,15 +3484,15 @@
         <v>39</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" s="37"/>
       <c r="D42" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E42" s="38"/>
       <c r="F42" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G42" s="38" t="s">
         <v>23</v>
@@ -3503,15 +3506,15 @@
         <v>39</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C43" s="37"/>
       <c r="D43" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E43" s="38"/>
       <c r="F43" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G43" s="38" t="s">
         <v>28</v>
@@ -3525,15 +3528,15 @@
         <v>39</v>
       </c>
       <c r="B44" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C44" s="37"/>
       <c r="D44" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E44" s="38"/>
       <c r="F44" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G44" s="38" t="s">
         <v>29</v>
@@ -3547,15 +3550,15 @@
         <v>39</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="37"/>
       <c r="D45" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E45" s="38"/>
       <c r="F45" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G45" s="38" t="s">
         <v>23</v>
@@ -3569,15 +3572,15 @@
         <v>39</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C46" s="37"/>
       <c r="D46" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E46" s="38"/>
       <c r="F46" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G46" s="38" t="s">
         <v>28</v>
@@ -3591,15 +3594,15 @@
         <v>39</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C47" s="37"/>
       <c r="D47" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E47" s="38"/>
       <c r="F47" s="38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G47" s="38" t="s">
         <v>23</v>
@@ -3613,15 +3616,15 @@
         <v>39</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48" s="37"/>
       <c r="D48" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E48" s="38"/>
       <c r="F48" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G48" s="38" t="s">
         <v>23</v>
@@ -3635,15 +3638,15 @@
         <v>39</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C49" s="37"/>
       <c r="D49" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E49" s="38"/>
       <c r="F49" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G49" s="38" t="s">
         <v>28</v>
@@ -3657,15 +3660,15 @@
         <v>39</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50" s="37"/>
       <c r="D50" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E50" s="38"/>
       <c r="F50" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G50" s="38" t="s">
         <v>23</v>
@@ -3679,15 +3682,15 @@
         <v>39</v>
       </c>
       <c r="B51" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C51" s="37"/>
       <c r="D51" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E51" s="38"/>
       <c r="F51" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G51" s="38" t="s">
         <v>28</v>
@@ -3701,15 +3704,15 @@
         <v>39</v>
       </c>
       <c r="B52" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C52" s="37"/>
       <c r="D52" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E52" s="38"/>
       <c r="F52" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G52" s="38" t="s">
         <v>23</v>
@@ -3723,15 +3726,15 @@
         <v>39</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C53" s="37"/>
       <c r="D53" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E53" s="38"/>
       <c r="F53" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G53" s="38" t="s">
         <v>23</v>
@@ -3745,15 +3748,15 @@
         <v>39</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E54" s="38"/>
       <c r="F54" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G54" s="38" t="s">
         <v>28</v>
@@ -3767,21 +3770,21 @@
         <v>39</v>
       </c>
       <c r="B55" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C55" s="37"/>
       <c r="D55" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E55" s="38"/>
       <c r="F55" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G55" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H55" s="39" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="I55" s="39" t="s">
         <v>33</v>
@@ -3795,21 +3798,21 @@
         <v>39</v>
       </c>
       <c r="B56" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C56" s="37"/>
       <c r="D56" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E56" s="38"/>
       <c r="F56" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G56" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H56" s="39" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="I56" s="39" t="s">
         <v>33</v>
@@ -3823,15 +3826,15 @@
         <v>39</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C57" s="37"/>
       <c r="D57" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E57" s="38"/>
       <c r="F57" s="38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G57" s="38" t="s">
         <v>23</v>
@@ -3845,15 +3848,15 @@
         <v>39</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E58" s="38"/>
       <c r="F58" s="38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G58" s="38" t="s">
         <v>28</v>
@@ -3867,15 +3870,15 @@
         <v>39</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C59" s="37"/>
       <c r="D59" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E59" s="38"/>
       <c r="F59" s="38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G59" s="38" t="s">
         <v>23</v>
@@ -3889,21 +3892,21 @@
         <v>39</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C60" s="37"/>
       <c r="D60" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E60" s="38"/>
       <c r="F60" s="38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G60" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H60" s="40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I60" s="39" t="s">
         <v>33</v>
@@ -3917,11 +3920,11 @@
         <v>39</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C61" s="37"/>
       <c r="D61" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E61" s="38" t="s">
         <v>23</v>
@@ -3937,15 +3940,15 @@
         <v>39</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C62" s="37"/>
       <c r="D62" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E62" s="38"/>
       <c r="F62" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G62" s="38" t="s">
         <v>23</v>
@@ -3959,15 +3962,15 @@
         <v>39</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E63" s="38"/>
       <c r="F63" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G63" s="38" t="s">
         <v>28</v>
@@ -3981,15 +3984,15 @@
         <v>39</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C64" s="37"/>
       <c r="D64" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E64" s="38"/>
       <c r="F64" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G64" s="38" t="s">
         <v>23</v>
@@ -4003,15 +4006,15 @@
         <v>39</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C65" s="37"/>
       <c r="D65" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E65" s="38"/>
       <c r="F65" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G65" s="38" t="s">
         <v>28</v>
@@ -4025,18 +4028,18 @@
         <v>39</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C66" s="37"/>
       <c r="D66" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E66" s="38"/>
       <c r="F66" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G66" s="38" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H66" s="40"/>
       <c r="I66" s="38"/>
@@ -4047,15 +4050,15 @@
         <v>39</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C67" s="37"/>
       <c r="D67" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E67" s="38"/>
       <c r="F67" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G67" s="38" t="s">
         <v>23</v>
@@ -4069,15 +4072,15 @@
         <v>39</v>
       </c>
       <c r="B68" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C68" s="37"/>
       <c r="D68" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E68" s="38"/>
       <c r="F68" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G68" s="38" t="s">
         <v>29</v>
@@ -4091,21 +4094,21 @@
         <v>39</v>
       </c>
       <c r="B69" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C69" s="37"/>
       <c r="D69" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E69" s="38"/>
       <c r="F69" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G69" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H69" s="40" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="I69" s="38" t="s">
         <v>33</v>
@@ -4119,15 +4122,15 @@
         <v>39</v>
       </c>
       <c r="B70" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C70" s="37"/>
       <c r="D70" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E70" s="38"/>
       <c r="F70" s="38" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G70" s="38" t="s">
         <v>23</v>
@@ -4141,15 +4144,15 @@
         <v>39</v>
       </c>
       <c r="B71" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C71" s="37"/>
       <c r="D71" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E71" s="38"/>
       <c r="F71" s="38" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G71" s="38" t="s">
         <v>28</v>
@@ -4163,15 +4166,15 @@
         <v>39</v>
       </c>
       <c r="B72" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C72" s="37"/>
       <c r="D72" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E72" s="38"/>
       <c r="F72" s="38" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G72" s="38" t="s">
         <v>24</v>
@@ -4185,15 +4188,15 @@
         <v>39</v>
       </c>
       <c r="B73" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C73" s="37"/>
       <c r="D73" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E73" s="38"/>
       <c r="F73" s="38" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G73" s="38" t="s">
         <v>23</v>
@@ -4207,15 +4210,15 @@
         <v>39</v>
       </c>
       <c r="B74" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C74" s="37"/>
       <c r="D74" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E74" s="38"/>
       <c r="F74" s="38" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G74" s="38" t="s">
         <v>28</v>
@@ -4229,15 +4232,15 @@
         <v>39</v>
       </c>
       <c r="B75" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C75" s="37"/>
       <c r="D75" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E75" s="38"/>
       <c r="F75" s="38" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G75" s="38" t="s">
         <v>23</v>
@@ -4251,15 +4254,15 @@
         <v>39</v>
       </c>
       <c r="B76" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C76" s="37"/>
       <c r="D76" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E76" s="38"/>
       <c r="F76" s="38" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G76" s="38" t="s">
         <v>23</v>
@@ -4273,15 +4276,15 @@
         <v>39</v>
       </c>
       <c r="B77" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C77" s="37"/>
       <c r="D77" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E77" s="38"/>
       <c r="F77" s="38" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G77" s="38" t="s">
         <v>24</v>
@@ -4295,21 +4298,21 @@
         <v>39</v>
       </c>
       <c r="B78" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C78" s="37"/>
       <c r="D78" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E78" s="38"/>
       <c r="F78" s="38" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G78" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H78" s="39" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I78" s="38" t="s">
         <v>33</v>
@@ -4323,7 +4326,7 @@
         <v>39</v>
       </c>
       <c r="B79" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C79" s="37"/>
       <c r="D79" s="38" t="s">
@@ -4343,7 +4346,7 @@
         <v>39</v>
       </c>
       <c r="B80" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C80" s="37"/>
       <c r="D80" s="38" t="s">
@@ -4355,7 +4358,7 @@
       <c r="F80" s="38"/>
       <c r="G80" s="38"/>
       <c r="H80" s="39" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I80" s="39" t="s">
         <v>33</v>
@@ -4369,7 +4372,7 @@
         <v>39</v>
       </c>
       <c r="B81" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C81" s="34" t="s">
         <v>23</v>
@@ -4387,7 +4390,7 @@
         <v>39</v>
       </c>
       <c r="B82" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C82" s="34" t="s">
         <v>29</v>
@@ -4405,7 +4408,7 @@
         <v>39</v>
       </c>
       <c r="B83" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C83" s="34" t="s">
         <v>23</v>
@@ -4423,11 +4426,11 @@
         <v>39</v>
       </c>
       <c r="B84" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C84" s="34"/>
       <c r="D84" s="41" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E84" s="41" t="s">
         <v>23</v>
@@ -4443,11 +4446,11 @@
         <v>39</v>
       </c>
       <c r="B85" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C85" s="34"/>
       <c r="D85" s="41" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E85" s="41" t="s">
         <v>28</v>
@@ -4463,11 +4466,11 @@
         <v>39</v>
       </c>
       <c r="B86" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C86" s="34"/>
       <c r="D86" s="41" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E86" s="41" t="s">
         <v>23</v>
@@ -4483,11 +4486,11 @@
         <v>39</v>
       </c>
       <c r="B87" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C87" s="34"/>
       <c r="D87" s="41" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E87" s="41" t="s">
         <v>28</v>
@@ -4503,11 +4506,11 @@
         <v>39</v>
       </c>
       <c r="B88" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C88" s="34"/>
       <c r="D88" s="41" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E88" s="41" t="s">
         <v>23</v>
@@ -4523,11 +4526,11 @@
         <v>39</v>
       </c>
       <c r="B89" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C89" s="34"/>
       <c r="D89" s="41" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E89" s="41" t="s">
         <v>23</v>
@@ -4543,7 +4546,7 @@
         <v>39</v>
       </c>
       <c r="B90" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C90" s="34"/>
       <c r="D90" s="41" t="s">
@@ -4563,7 +4566,7 @@
         <v>39</v>
       </c>
       <c r="B91" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C91" s="34"/>
       <c r="D91" s="41" t="s">
@@ -4575,7 +4578,7 @@
       <c r="F91" s="41"/>
       <c r="G91" s="41"/>
       <c r="H91" s="42" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I91" s="42" t="s">
         <v>33</v>
@@ -4589,7 +4592,7 @@
         <v>39</v>
       </c>
       <c r="B92" s="33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C92" s="43" t="s">
         <v>23</v>
@@ -4607,7 +4610,7 @@
         <v>39</v>
       </c>
       <c r="B93" s="33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C93" s="47" t="s">
         <v>28</v>
@@ -4625,7 +4628,7 @@
         <v>39</v>
       </c>
       <c r="B94" s="33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C94" s="46" t="s">
         <v>23</v>
@@ -4643,7 +4646,7 @@
         <v>39</v>
       </c>
       <c r="B95" s="33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C95" s="46"/>
       <c r="D95" s="44" t="s">
@@ -4663,7 +4666,7 @@
         <v>39</v>
       </c>
       <c r="B96" s="33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C96" s="46"/>
       <c r="D96" s="44" t="s">
@@ -4675,7 +4678,7 @@
       <c r="F96" s="44"/>
       <c r="G96" s="44"/>
       <c r="H96" s="45" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I96" s="45" t="s">
         <v>33</v>
@@ -4717,7 +4720,7 @@
       <c r="F98" s="48"/>
       <c r="G98" s="48"/>
       <c r="H98" s="49" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I98" s="49" t="s">
         <v>34</v>
@@ -4741,7 +4744,7 @@
       <c r="F99" s="48"/>
       <c r="G99" s="48"/>
       <c r="H99" s="49" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I99" s="49" t="s">
         <v>33</v>
@@ -4755,7 +4758,7 @@
         <v>39</v>
       </c>
       <c r="B100" s="34" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C100" s="34" t="s">
         <v>22</v>
@@ -4777,10 +4780,10 @@
         <v>39</v>
       </c>
       <c r="B101" s="34" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C101" s="34" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D101" s="41"/>
       <c r="E101" s="41"/>

</xml_diff>

<commit_message>
Revert "GUION 3 GRADO 8 DEFINITIVOS"
This reverts commit 9992c8c021ad41506b86bf40ba23afc3e3da6514.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/EsqueletoGuion_CS_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/EsqueletoGuion_CS_08_02_CO.xlsx
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'CUADERNO DEL PROFESOR'!$C$1:$C$30</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="105">
   <si>
     <t>FICHA</t>
   </si>
@@ -160,6 +160,9 @@
     <t>Reformas administrativas y económicas</t>
   </si>
   <si>
+    <t>Practica: Los virreinatos españoles en América</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reforma eclesiástica </t>
   </si>
   <si>
@@ -226,6 +229,9 @@
     <t>La creación de Bolivia</t>
   </si>
   <si>
+    <t>Practica: Las batallas que definieron la Independencia</t>
+  </si>
+  <si>
     <t>Independencia del Río de la Plata</t>
   </si>
   <si>
@@ -235,12 +241,18 @@
     <t>Encuentra el hecho o el personaje de la Independencia</t>
   </si>
   <si>
+    <t>Refuerza tu aprendizaje: Conoce el pensamiento de Simón Bolívar</t>
+  </si>
+  <si>
     <t>Independencia de las colonias de Centroamérica</t>
   </si>
   <si>
     <t>El Grito de Dolores, en México</t>
   </si>
   <si>
+    <t>Practica: Los principios del Plan de Iguala</t>
+  </si>
+  <si>
     <t>Independencia de El Salvador</t>
   </si>
   <si>
@@ -268,6 +280,9 @@
     <t>Refuerza tu aprendizaje: Los caudillos</t>
   </si>
   <si>
+    <t>Practica: La independencia de Centroamérica</t>
+  </si>
+  <si>
     <t>Manifestaciones artísticas y culturales</t>
   </si>
   <si>
@@ -322,31 +337,13 @@
     <t>Refuerza tu aprendizaje: La Independencia centroamericana</t>
   </si>
   <si>
+    <t>Practica: La Independencia de Centroamérica</t>
+  </si>
+  <si>
     <t>La Independencia de las colonias americanas</t>
   </si>
   <si>
-    <t>Competencias: Cronología de la Independencia americana</t>
-  </si>
-  <si>
-    <t>Los virreinatos españoles en América</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Los virreinatos españoles en América</t>
-  </si>
-  <si>
-    <t>Simón Bolívar y la Independencia</t>
-  </si>
-  <si>
-    <t>Los principios del Plan de Iguala</t>
-  </si>
-  <si>
-    <t>Las batallas que definieron la Independencia</t>
-  </si>
-  <si>
-    <t>La Independencia de Centroamérica</t>
-  </si>
-  <si>
-    <t>La independencia de Centroamérica</t>
+    <t>Competencias: cronología de la Independencia americana</t>
   </si>
 </sst>
 </file>
@@ -1879,19 +1876,19 @@
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1907,19 +1904,19 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1927,19 +1924,19 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -1947,19 +1944,19 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F5">
         <v>9</v>
@@ -1967,19 +1964,19 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" t="s">
         <v>98</v>
-      </c>
-      <c r="E6" t="s">
-        <v>93</v>
       </c>
       <c r="F6">
         <v>18</v>
@@ -2001,7 +1998,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2023,7 +2020,7 @@
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="B2" s="54" t="s">
         <v>33</v>
@@ -2035,7 +2032,7 @@
     </row>
     <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="54" t="s">
         <v>33</v>
@@ -2047,7 +2044,7 @@
     </row>
     <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="54" t="s">
         <v>33</v>
@@ -2059,7 +2056,7 @@
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B5" s="54" t="s">
         <v>33</v>
@@ -2070,7 +2067,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B6" s="54" t="s">
         <v>33</v>
@@ -2081,7 +2078,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="B7" s="54" t="s">
         <v>33</v>
@@ -2092,7 +2089,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="B8" s="54" t="s">
         <v>33</v>
@@ -2103,7 +2100,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B9" s="54" t="s">
         <v>33</v>
@@ -2114,7 +2111,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B10" s="54" t="s">
         <v>33</v>
@@ -2125,7 +2122,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="B11" s="54" t="s">
         <v>33</v>
@@ -2136,7 +2133,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B12" s="54" t="s">
         <v>33</v>
@@ -2147,7 +2144,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B13" s="54" t="s">
         <v>33</v>
@@ -2158,7 +2155,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B14" s="54" t="s">
         <v>33</v>
@@ -2169,7 +2166,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B15" s="54" t="s">
         <v>33</v>
@@ -2235,7 +2232,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,7 +2270,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="C3" s="51" t="s">
         <v>33</v>
@@ -2285,7 +2282,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C4" s="53" t="s">
         <v>34</v>
@@ -2297,7 +2294,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C5" s="51" t="s">
         <v>33</v>
@@ -2309,7 +2306,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C6" s="53" t="s">
         <v>34</v>
@@ -2321,7 +2318,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C7" s="51" t="s">
         <v>33</v>
@@ -2333,7 +2330,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C8" s="51" t="s">
         <v>33</v>
@@ -2345,7 +2342,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C9" s="51" t="s">
         <v>33</v>
@@ -2357,7 +2354,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C10" s="53" t="s">
         <v>34</v>
@@ -2369,7 +2366,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="C11" s="51" t="s">
         <v>33</v>
@@ -2381,7 +2378,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="C12" s="51" t="s">
         <v>33</v>
@@ -2393,7 +2390,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C13" s="51" t="s">
         <v>33</v>
@@ -2405,7 +2402,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="C14" s="53" t="s">
         <v>34</v>
@@ -2417,7 +2414,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C15" s="51" t="s">
         <v>33</v>
@@ -2429,7 +2426,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C16" s="53" t="s">
         <v>34</v>
@@ -2441,7 +2438,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C17" s="51" t="s">
         <v>33</v>
@@ -2453,7 +2450,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C18" s="51" t="s">
         <v>33</v>
@@ -2465,7 +2462,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="52" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C19" s="53" t="s">
         <v>34</v>
@@ -2477,7 +2474,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C20" s="53" t="s">
         <v>33</v>
@@ -2561,8 +2558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D76" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="H99" sqref="H99"/>
+    <sheetView tabSelected="1" topLeftCell="E49" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2614,7 +2611,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>23</v>
@@ -2632,7 +2629,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>28</v>
@@ -2650,7 +2647,7 @@
         <v>39</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>24</v>
@@ -2668,7 +2665,7 @@
         <v>39</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="20" t="s">
@@ -2688,7 +2685,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="20" t="s">
@@ -2708,7 +2705,7 @@
         <v>39</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="20" t="s">
@@ -2728,7 +2725,7 @@
         <v>39</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="20" t="s">
@@ -2754,7 +2751,7 @@
         <v>39</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="20" t="s">
@@ -2776,7 +2773,7 @@
         <v>39</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="20" t="s">
@@ -2790,7 +2787,7 @@
         <v>26</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="I10" s="21" t="s">
         <v>33</v>
@@ -2804,7 +2801,7 @@
         <v>39</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="20" t="s">
@@ -2826,7 +2823,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="20" t="s">
@@ -2848,7 +2845,7 @@
         <v>39</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="20" t="s">
@@ -2856,7 +2853,7 @@
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>23</v>
@@ -2870,7 +2867,7 @@
         <v>39</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="20" t="s">
@@ -2878,7 +2875,7 @@
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>28</v>
@@ -2892,7 +2889,7 @@
         <v>39</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="20" t="s">
@@ -2900,7 +2897,7 @@
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>23</v>
@@ -2914,7 +2911,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="20" t="s">
@@ -2922,7 +2919,7 @@
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>24</v>
@@ -2936,7 +2933,7 @@
         <v>39</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="20" t="s">
@@ -2944,13 +2941,13 @@
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>34</v>
@@ -2964,7 +2961,7 @@
         <v>39</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="20" t="s">
@@ -2972,13 +2969,13 @@
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>33</v>
@@ -2992,11 +2989,11 @@
         <v>39</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>23</v>
@@ -3012,11 +3009,11 @@
         <v>39</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>23</v>
@@ -3032,11 +3029,11 @@
         <v>39</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>28</v>
@@ -3052,11 +3049,11 @@
         <v>39</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C22" s="23"/>
       <c r="D22" s="20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>23</v>
@@ -3072,11 +3069,11 @@
         <v>39</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>28</v>
@@ -3092,11 +3089,11 @@
         <v>39</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E24" s="20" t="s">
         <v>27</v>
@@ -3104,7 +3101,7 @@
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I24" s="21" t="s">
         <v>34</v>
@@ -3118,11 +3115,11 @@
         <v>39</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>23</v>
@@ -3138,11 +3135,11 @@
         <v>39</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C26" s="23"/>
       <c r="D26" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>26</v>
@@ -3150,7 +3147,7 @@
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I26" s="21" t="s">
         <v>33</v>
@@ -3164,11 +3161,11 @@
         <v>39</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C27" s="23"/>
       <c r="D27" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>29</v>
@@ -3184,11 +3181,11 @@
         <v>39</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>24</v>
@@ -3204,7 +3201,7 @@
         <v>39</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C29" s="23"/>
       <c r="D29" s="20" t="s">
@@ -3224,7 +3221,7 @@
         <v>39</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="20" t="s">
@@ -3236,7 +3233,7 @@
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
       <c r="H30" s="21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I30" s="21" t="s">
         <v>33</v>
@@ -3250,7 +3247,7 @@
         <v>39</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C31" s="37" t="s">
         <v>23</v>
@@ -3268,11 +3265,11 @@
         <v>39</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C32" s="37"/>
       <c r="D32" s="38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E32" s="38" t="s">
         <v>23</v>
@@ -3288,11 +3285,11 @@
         <v>39</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C33" s="37"/>
       <c r="D33" s="38" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E33" s="38" t="s">
         <v>23</v>
@@ -3308,11 +3305,11 @@
         <v>39</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C34" s="37"/>
       <c r="D34" s="38" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E34" s="38" t="s">
         <v>28</v>
@@ -3328,11 +3325,11 @@
         <v>39</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C35" s="37"/>
       <c r="D35" s="38" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E35" s="38" t="s">
         <v>23</v>
@@ -3348,11 +3345,11 @@
         <v>39</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C36" s="37"/>
       <c r="D36" s="38" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E36" s="38" t="s">
         <v>28</v>
@@ -3368,11 +3365,11 @@
         <v>39</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C37" s="37"/>
       <c r="D37" s="38" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E37" s="38" t="s">
         <v>26</v>
@@ -3380,7 +3377,7 @@
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
       <c r="H37" s="39" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I37" s="39" t="s">
         <v>33</v>
@@ -3394,11 +3391,11 @@
         <v>39</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C38" s="37"/>
       <c r="D38" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E38" s="38" t="s">
         <v>23</v>
@@ -3414,11 +3411,11 @@
         <v>39</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C39" s="37"/>
       <c r="D39" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E39" s="38" t="s">
         <v>27</v>
@@ -3426,7 +3423,7 @@
       <c r="F39" s="38"/>
       <c r="G39" s="38"/>
       <c r="H39" s="40" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="I39" s="38" t="s">
         <v>34</v>
@@ -3440,15 +3437,15 @@
         <v>39</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C40" s="37"/>
       <c r="D40" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E40" s="38"/>
       <c r="F40" s="38" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G40" s="38" t="s">
         <v>23</v>
@@ -3462,15 +3459,15 @@
         <v>39</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C41" s="37"/>
       <c r="D41" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E41" s="38"/>
       <c r="F41" s="38" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G41" s="38" t="s">
         <v>28</v>
@@ -3484,15 +3481,15 @@
         <v>39</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C42" s="37"/>
       <c r="D42" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E42" s="38"/>
       <c r="F42" s="38" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G42" s="38" t="s">
         <v>23</v>
@@ -3506,15 +3503,15 @@
         <v>39</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C43" s="37"/>
       <c r="D43" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E43" s="38"/>
       <c r="F43" s="38" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G43" s="38" t="s">
         <v>28</v>
@@ -3528,15 +3525,15 @@
         <v>39</v>
       </c>
       <c r="B44" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C44" s="37"/>
       <c r="D44" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E44" s="38"/>
       <c r="F44" s="38" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G44" s="38" t="s">
         <v>29</v>
@@ -3550,15 +3547,15 @@
         <v>39</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C45" s="37"/>
       <c r="D45" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E45" s="38"/>
       <c r="F45" s="38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G45" s="38" t="s">
         <v>23</v>
@@ -3572,15 +3569,15 @@
         <v>39</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C46" s="37"/>
       <c r="D46" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E46" s="38"/>
       <c r="F46" s="38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G46" s="38" t="s">
         <v>28</v>
@@ -3594,15 +3591,15 @@
         <v>39</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C47" s="37"/>
       <c r="D47" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E47" s="38"/>
       <c r="F47" s="38" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G47" s="38" t="s">
         <v>23</v>
@@ -3616,15 +3613,15 @@
         <v>39</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C48" s="37"/>
       <c r="D48" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E48" s="38"/>
       <c r="F48" s="38" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G48" s="38" t="s">
         <v>23</v>
@@ -3638,15 +3635,15 @@
         <v>39</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C49" s="37"/>
       <c r="D49" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E49" s="38"/>
       <c r="F49" s="38" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G49" s="38" t="s">
         <v>28</v>
@@ -3660,15 +3657,15 @@
         <v>39</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C50" s="37"/>
       <c r="D50" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E50" s="38"/>
       <c r="F50" s="38" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G50" s="38" t="s">
         <v>23</v>
@@ -3682,15 +3679,15 @@
         <v>39</v>
       </c>
       <c r="B51" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C51" s="37"/>
       <c r="D51" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E51" s="38"/>
       <c r="F51" s="38" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G51" s="38" t="s">
         <v>28</v>
@@ -3704,15 +3701,15 @@
         <v>39</v>
       </c>
       <c r="B52" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C52" s="37"/>
       <c r="D52" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E52" s="38"/>
       <c r="F52" s="38" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G52" s="38" t="s">
         <v>23</v>
@@ -3726,15 +3723,15 @@
         <v>39</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C53" s="37"/>
       <c r="D53" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E53" s="38"/>
       <c r="F53" s="38" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G53" s="38" t="s">
         <v>23</v>
@@ -3748,15 +3745,15 @@
         <v>39</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E54" s="38"/>
       <c r="F54" s="38" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G54" s="38" t="s">
         <v>28</v>
@@ -3770,21 +3767,21 @@
         <v>39</v>
       </c>
       <c r="B55" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C55" s="37"/>
       <c r="D55" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E55" s="38"/>
       <c r="F55" s="38" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G55" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H55" s="39" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="I55" s="39" t="s">
         <v>33</v>
@@ -3798,21 +3795,21 @@
         <v>39</v>
       </c>
       <c r="B56" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C56" s="37"/>
       <c r="D56" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E56" s="38"/>
       <c r="F56" s="38" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G56" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H56" s="39" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="I56" s="39" t="s">
         <v>33</v>
@@ -3826,15 +3823,15 @@
         <v>39</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C57" s="37"/>
       <c r="D57" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E57" s="38"/>
       <c r="F57" s="38" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G57" s="38" t="s">
         <v>23</v>
@@ -3848,15 +3845,15 @@
         <v>39</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E58" s="38"/>
       <c r="F58" s="38" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G58" s="38" t="s">
         <v>28</v>
@@ -3870,15 +3867,15 @@
         <v>39</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C59" s="37"/>
       <c r="D59" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E59" s="38"/>
       <c r="F59" s="38" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G59" s="38" t="s">
         <v>23</v>
@@ -3892,21 +3889,21 @@
         <v>39</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C60" s="37"/>
       <c r="D60" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E60" s="38"/>
       <c r="F60" s="38" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G60" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H60" s="40" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I60" s="39" t="s">
         <v>33</v>
@@ -3920,11 +3917,11 @@
         <v>39</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C61" s="37"/>
       <c r="D61" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E61" s="38" t="s">
         <v>23</v>
@@ -3940,15 +3937,15 @@
         <v>39</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C62" s="37"/>
       <c r="D62" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E62" s="38"/>
       <c r="F62" s="38" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G62" s="38" t="s">
         <v>23</v>
@@ -3962,15 +3959,15 @@
         <v>39</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E63" s="38"/>
       <c r="F63" s="38" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G63" s="38" t="s">
         <v>28</v>
@@ -3984,15 +3981,15 @@
         <v>39</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C64" s="37"/>
       <c r="D64" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E64" s="38"/>
       <c r="F64" s="38" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G64" s="38" t="s">
         <v>23</v>
@@ -4006,15 +4003,15 @@
         <v>39</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C65" s="37"/>
       <c r="D65" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E65" s="38"/>
       <c r="F65" s="38" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G65" s="38" t="s">
         <v>28</v>
@@ -4028,18 +4025,18 @@
         <v>39</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C66" s="37"/>
       <c r="D66" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E66" s="38"/>
       <c r="F66" s="38" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G66" s="38" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H66" s="40"/>
       <c r="I66" s="38"/>
@@ -4050,15 +4047,15 @@
         <v>39</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C67" s="37"/>
       <c r="D67" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E67" s="38"/>
       <c r="F67" s="38" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G67" s="38" t="s">
         <v>23</v>
@@ -4072,15 +4069,15 @@
         <v>39</v>
       </c>
       <c r="B68" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C68" s="37"/>
       <c r="D68" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E68" s="38"/>
       <c r="F68" s="38" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G68" s="38" t="s">
         <v>29</v>
@@ -4094,21 +4091,21 @@
         <v>39</v>
       </c>
       <c r="B69" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C69" s="37"/>
       <c r="D69" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E69" s="38"/>
       <c r="F69" s="38" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G69" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H69" s="40" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="I69" s="38" t="s">
         <v>33</v>
@@ -4122,15 +4119,15 @@
         <v>39</v>
       </c>
       <c r="B70" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C70" s="37"/>
       <c r="D70" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E70" s="38"/>
       <c r="F70" s="38" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G70" s="38" t="s">
         <v>23</v>
@@ -4144,15 +4141,15 @@
         <v>39</v>
       </c>
       <c r="B71" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C71" s="37"/>
       <c r="D71" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E71" s="38"/>
       <c r="F71" s="38" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G71" s="38" t="s">
         <v>28</v>
@@ -4166,15 +4163,15 @@
         <v>39</v>
       </c>
       <c r="B72" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C72" s="37"/>
       <c r="D72" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E72" s="38"/>
       <c r="F72" s="38" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G72" s="38" t="s">
         <v>24</v>
@@ -4188,15 +4185,15 @@
         <v>39</v>
       </c>
       <c r="B73" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C73" s="37"/>
       <c r="D73" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E73" s="38"/>
       <c r="F73" s="38" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G73" s="38" t="s">
         <v>23</v>
@@ -4210,15 +4207,15 @@
         <v>39</v>
       </c>
       <c r="B74" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C74" s="37"/>
       <c r="D74" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E74" s="38"/>
       <c r="F74" s="38" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G74" s="38" t="s">
         <v>28</v>
@@ -4232,15 +4229,15 @@
         <v>39</v>
       </c>
       <c r="B75" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C75" s="37"/>
       <c r="D75" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E75" s="38"/>
       <c r="F75" s="38" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G75" s="38" t="s">
         <v>23</v>
@@ -4254,15 +4251,15 @@
         <v>39</v>
       </c>
       <c r="B76" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C76" s="37"/>
       <c r="D76" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E76" s="38"/>
       <c r="F76" s="38" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G76" s="38" t="s">
         <v>23</v>
@@ -4276,15 +4273,15 @@
         <v>39</v>
       </c>
       <c r="B77" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C77" s="37"/>
       <c r="D77" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E77" s="38"/>
       <c r="F77" s="38" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G77" s="38" t="s">
         <v>24</v>
@@ -4298,21 +4295,21 @@
         <v>39</v>
       </c>
       <c r="B78" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C78" s="37"/>
       <c r="D78" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E78" s="38"/>
       <c r="F78" s="38" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G78" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H78" s="39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I78" s="38" t="s">
         <v>33</v>
@@ -4326,7 +4323,7 @@
         <v>39</v>
       </c>
       <c r="B79" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C79" s="37"/>
       <c r="D79" s="38" t="s">
@@ -4346,7 +4343,7 @@
         <v>39</v>
       </c>
       <c r="B80" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C80" s="37"/>
       <c r="D80" s="38" t="s">
@@ -4358,7 +4355,7 @@
       <c r="F80" s="38"/>
       <c r="G80" s="38"/>
       <c r="H80" s="39" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I80" s="39" t="s">
         <v>33</v>
@@ -4372,7 +4369,7 @@
         <v>39</v>
       </c>
       <c r="B81" s="34" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C81" s="34" t="s">
         <v>23</v>
@@ -4390,7 +4387,7 @@
         <v>39</v>
       </c>
       <c r="B82" s="34" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C82" s="34" t="s">
         <v>29</v>
@@ -4408,7 +4405,7 @@
         <v>39</v>
       </c>
       <c r="B83" s="34" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C83" s="34" t="s">
         <v>23</v>
@@ -4426,11 +4423,11 @@
         <v>39</v>
       </c>
       <c r="B84" s="34" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C84" s="34"/>
       <c r="D84" s="41" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E84" s="41" t="s">
         <v>23</v>
@@ -4446,11 +4443,11 @@
         <v>39</v>
       </c>
       <c r="B85" s="34" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C85" s="34"/>
       <c r="D85" s="41" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E85" s="41" t="s">
         <v>28</v>
@@ -4466,11 +4463,11 @@
         <v>39</v>
       </c>
       <c r="B86" s="34" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C86" s="34"/>
       <c r="D86" s="41" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E86" s="41" t="s">
         <v>23</v>
@@ -4486,11 +4483,11 @@
         <v>39</v>
       </c>
       <c r="B87" s="34" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C87" s="34"/>
       <c r="D87" s="41" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E87" s="41" t="s">
         <v>28</v>
@@ -4506,11 +4503,11 @@
         <v>39</v>
       </c>
       <c r="B88" s="34" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C88" s="34"/>
       <c r="D88" s="41" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E88" s="41" t="s">
         <v>23</v>
@@ -4526,11 +4523,11 @@
         <v>39</v>
       </c>
       <c r="B89" s="34" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C89" s="34"/>
       <c r="D89" s="41" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E89" s="41" t="s">
         <v>23</v>
@@ -4546,7 +4543,7 @@
         <v>39</v>
       </c>
       <c r="B90" s="34" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C90" s="34"/>
       <c r="D90" s="41" t="s">
@@ -4566,7 +4563,7 @@
         <v>39</v>
       </c>
       <c r="B91" s="34" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C91" s="34"/>
       <c r="D91" s="41" t="s">
@@ -4578,7 +4575,7 @@
       <c r="F91" s="41"/>
       <c r="G91" s="41"/>
       <c r="H91" s="42" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="I91" s="42" t="s">
         <v>33</v>
@@ -4592,7 +4589,7 @@
         <v>39</v>
       </c>
       <c r="B92" s="33" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C92" s="43" t="s">
         <v>23</v>
@@ -4610,7 +4607,7 @@
         <v>39</v>
       </c>
       <c r="B93" s="33" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C93" s="47" t="s">
         <v>28</v>
@@ -4628,7 +4625,7 @@
         <v>39</v>
       </c>
       <c r="B94" s="33" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C94" s="46" t="s">
         <v>23</v>
@@ -4646,7 +4643,7 @@
         <v>39</v>
       </c>
       <c r="B95" s="33" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C95" s="46"/>
       <c r="D95" s="44" t="s">
@@ -4666,7 +4663,7 @@
         <v>39</v>
       </c>
       <c r="B96" s="33" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C96" s="46"/>
       <c r="D96" s="44" t="s">
@@ -4678,7 +4675,7 @@
       <c r="F96" s="44"/>
       <c r="G96" s="44"/>
       <c r="H96" s="45" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="I96" s="45" t="s">
         <v>33</v>
@@ -4720,7 +4717,7 @@
       <c r="F98" s="48"/>
       <c r="G98" s="48"/>
       <c r="H98" s="49" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I98" s="49" t="s">
         <v>34</v>
@@ -4744,7 +4741,7 @@
       <c r="F99" s="48"/>
       <c r="G99" s="48"/>
       <c r="H99" s="49" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I99" s="49" t="s">
         <v>33</v>
@@ -4758,7 +4755,7 @@
         <v>39</v>
       </c>
       <c r="B100" s="34" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C100" s="34" t="s">
         <v>22</v>
@@ -4780,10 +4777,10 @@
         <v>39</v>
       </c>
       <c r="B101" s="34" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C101" s="34" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D101" s="41"/>
       <c r="E101" s="41"/>

</xml_diff>

<commit_message>
Revert "Revert "GUION 3 GRADO 8 DEFINITIVOS""
This reverts commit 2b10ab14e662f545f192101344b3168707e42cce.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/EsqueletoGuion_CS_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/EsqueletoGuion_CS_08_02_CO.xlsx
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'CUADERNO DEL PROFESOR'!$C$1:$C$30</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="106">
   <si>
     <t>FICHA</t>
   </si>
@@ -160,9 +160,6 @@
     <t>Reformas administrativas y económicas</t>
   </si>
   <si>
-    <t>Practica: Los virreinatos españoles en América</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reforma eclesiástica </t>
   </si>
   <si>
@@ -229,9 +226,6 @@
     <t>La creación de Bolivia</t>
   </si>
   <si>
-    <t>Practica: Las batallas que definieron la Independencia</t>
-  </si>
-  <si>
     <t>Independencia del Río de la Plata</t>
   </si>
   <si>
@@ -241,18 +235,12 @@
     <t>Encuentra el hecho o el personaje de la Independencia</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Conoce el pensamiento de Simón Bolívar</t>
-  </si>
-  <si>
     <t>Independencia de las colonias de Centroamérica</t>
   </si>
   <si>
     <t>El Grito de Dolores, en México</t>
   </si>
   <si>
-    <t>Practica: Los principios del Plan de Iguala</t>
-  </si>
-  <si>
     <t>Independencia de El Salvador</t>
   </si>
   <si>
@@ -280,9 +268,6 @@
     <t>Refuerza tu aprendizaje: Los caudillos</t>
   </si>
   <si>
-    <t>Practica: La independencia de Centroamérica</t>
-  </si>
-  <si>
     <t>Manifestaciones artísticas y culturales</t>
   </si>
   <si>
@@ -337,13 +322,31 @@
     <t>Refuerza tu aprendizaje: La Independencia centroamericana</t>
   </si>
   <si>
-    <t>Practica: La Independencia de Centroamérica</t>
-  </si>
-  <si>
     <t>La Independencia de las colonias americanas</t>
   </si>
   <si>
-    <t>Competencias: cronología de la Independencia americana</t>
+    <t>Competencias: Cronología de la Independencia americana</t>
+  </si>
+  <si>
+    <t>Los virreinatos españoles en América</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Los virreinatos españoles en América</t>
+  </si>
+  <si>
+    <t>Simón Bolívar y la Independencia</t>
+  </si>
+  <si>
+    <t>Los principios del Plan de Iguala</t>
+  </si>
+  <si>
+    <t>Las batallas que definieron la Independencia</t>
+  </si>
+  <si>
+    <t>La Independencia de Centroamérica</t>
+  </si>
+  <si>
+    <t>La independencia de Centroamérica</t>
   </si>
 </sst>
 </file>
@@ -1876,19 +1879,19 @@
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1904,19 +1907,19 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1924,19 +1927,19 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
         <v>93</v>
-      </c>
-      <c r="C4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" t="s">
-        <v>98</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -1944,19 +1947,19 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
         <v>93</v>
-      </c>
-      <c r="C5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E5" t="s">
-        <v>98</v>
       </c>
       <c r="F5">
         <v>9</v>
@@ -1964,19 +1967,19 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
         <v>93</v>
-      </c>
-      <c r="C6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" t="s">
-        <v>98</v>
       </c>
       <c r="F6">
         <v>18</v>
@@ -1998,7 +2001,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2020,7 +2023,7 @@
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="B2" s="54" t="s">
         <v>33</v>
@@ -2032,7 +2035,7 @@
     </row>
     <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="54" t="s">
         <v>33</v>
@@ -2044,7 +2047,7 @@
     </row>
     <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="54" t="s">
         <v>33</v>
@@ -2056,7 +2059,7 @@
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="54" t="s">
         <v>33</v>
@@ -2067,7 +2070,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="54" t="s">
         <v>33</v>
@@ -2078,7 +2081,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="B7" s="54" t="s">
         <v>33</v>
@@ -2089,7 +2092,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="B8" s="54" t="s">
         <v>33</v>
@@ -2100,7 +2103,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" s="54" t="s">
         <v>33</v>
@@ -2111,7 +2114,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="B10" s="54" t="s">
         <v>33</v>
@@ -2122,7 +2125,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="B11" s="54" t="s">
         <v>33</v>
@@ -2133,7 +2136,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B12" s="54" t="s">
         <v>33</v>
@@ -2144,7 +2147,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B13" s="54" t="s">
         <v>33</v>
@@ -2155,7 +2158,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B14" s="54" t="s">
         <v>33</v>
@@ -2166,7 +2169,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B15" s="54" t="s">
         <v>33</v>
@@ -2232,7 +2235,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2270,7 +2273,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="C3" s="51" t="s">
         <v>33</v>
@@ -2282,7 +2285,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="53" t="s">
         <v>34</v>
@@ -2294,7 +2297,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="51" t="s">
         <v>33</v>
@@ -2306,7 +2309,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="53" t="s">
         <v>34</v>
@@ -2318,7 +2321,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="51" t="s">
         <v>33</v>
@@ -2330,7 +2333,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="51" t="s">
         <v>33</v>
@@ -2342,7 +2345,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="51" t="s">
         <v>33</v>
@@ -2354,7 +2357,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C10" s="53" t="s">
         <v>34</v>
@@ -2366,7 +2369,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="C11" s="51" t="s">
         <v>33</v>
@@ -2378,7 +2381,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="C12" s="51" t="s">
         <v>33</v>
@@ -2390,7 +2393,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C13" s="51" t="s">
         <v>33</v>
@@ -2402,7 +2405,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="C14" s="53" t="s">
         <v>34</v>
@@ -2414,7 +2417,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C15" s="51" t="s">
         <v>33</v>
@@ -2426,7 +2429,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C16" s="53" t="s">
         <v>34</v>
@@ -2438,7 +2441,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C17" s="51" t="s">
         <v>33</v>
@@ -2450,7 +2453,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C18" s="51" t="s">
         <v>33</v>
@@ -2462,7 +2465,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="52" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C19" s="53" t="s">
         <v>34</v>
@@ -2474,7 +2477,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C20" s="53" t="s">
         <v>33</v>
@@ -2558,8 +2561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E49" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="D76" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="H99" sqref="H99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2611,7 +2614,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>23</v>
@@ -2629,7 +2632,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>28</v>
@@ -2647,7 +2650,7 @@
         <v>39</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>24</v>
@@ -2665,7 +2668,7 @@
         <v>39</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="20" t="s">
@@ -2685,7 +2688,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="20" t="s">
@@ -2705,7 +2708,7 @@
         <v>39</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="20" t="s">
@@ -2725,7 +2728,7 @@
         <v>39</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="20" t="s">
@@ -2751,7 +2754,7 @@
         <v>39</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="20" t="s">
@@ -2773,7 +2776,7 @@
         <v>39</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="20" t="s">
@@ -2787,7 +2790,7 @@
         <v>26</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="I10" s="21" t="s">
         <v>33</v>
@@ -2801,7 +2804,7 @@
         <v>39</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="20" t="s">
@@ -2823,7 +2826,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="20" t="s">
@@ -2845,7 +2848,7 @@
         <v>39</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="20" t="s">
@@ -2853,7 +2856,7 @@
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>23</v>
@@ -2867,7 +2870,7 @@
         <v>39</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="20" t="s">
@@ -2875,7 +2878,7 @@
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>28</v>
@@ -2889,7 +2892,7 @@
         <v>39</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="20" t="s">
@@ -2897,7 +2900,7 @@
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>23</v>
@@ -2911,7 +2914,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="20" t="s">
@@ -2919,7 +2922,7 @@
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>24</v>
@@ -2933,7 +2936,7 @@
         <v>39</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="20" t="s">
@@ -2941,13 +2944,13 @@
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>34</v>
@@ -2961,7 +2964,7 @@
         <v>39</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="20" t="s">
@@ -2969,13 +2972,13 @@
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>33</v>
@@ -2989,11 +2992,11 @@
         <v>39</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>23</v>
@@ -3009,11 +3012,11 @@
         <v>39</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>23</v>
@@ -3029,11 +3032,11 @@
         <v>39</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>28</v>
@@ -3049,11 +3052,11 @@
         <v>39</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C22" s="23"/>
       <c r="D22" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>23</v>
@@ -3069,11 +3072,11 @@
         <v>39</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>28</v>
@@ -3089,11 +3092,11 @@
         <v>39</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="20" t="s">
         <v>27</v>
@@ -3101,7 +3104,7 @@
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I24" s="21" t="s">
         <v>34</v>
@@ -3115,11 +3118,11 @@
         <v>39</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>23</v>
@@ -3135,11 +3138,11 @@
         <v>39</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C26" s="23"/>
       <c r="D26" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>26</v>
@@ -3147,7 +3150,7 @@
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I26" s="21" t="s">
         <v>33</v>
@@ -3161,11 +3164,11 @@
         <v>39</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C27" s="23"/>
       <c r="D27" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>29</v>
@@ -3181,11 +3184,11 @@
         <v>39</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>24</v>
@@ -3201,7 +3204,7 @@
         <v>39</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C29" s="23"/>
       <c r="D29" s="20" t="s">
@@ -3221,7 +3224,7 @@
         <v>39</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="20" t="s">
@@ -3233,7 +3236,7 @@
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
       <c r="H30" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I30" s="21" t="s">
         <v>33</v>
@@ -3247,7 +3250,7 @@
         <v>39</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="37" t="s">
         <v>23</v>
@@ -3265,11 +3268,11 @@
         <v>39</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="37"/>
       <c r="D32" s="38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E32" s="38" t="s">
         <v>23</v>
@@ -3285,11 +3288,11 @@
         <v>39</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="37"/>
       <c r="D33" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E33" s="38" t="s">
         <v>23</v>
@@ -3305,11 +3308,11 @@
         <v>39</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="37"/>
       <c r="D34" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E34" s="38" t="s">
         <v>28</v>
@@ -3325,11 +3328,11 @@
         <v>39</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" s="37"/>
       <c r="D35" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E35" s="38" t="s">
         <v>23</v>
@@ -3345,11 +3348,11 @@
         <v>39</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" s="37"/>
       <c r="D36" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E36" s="38" t="s">
         <v>28</v>
@@ -3365,11 +3368,11 @@
         <v>39</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C37" s="37"/>
       <c r="D37" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E37" s="38" t="s">
         <v>26</v>
@@ -3377,7 +3380,7 @@
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
       <c r="H37" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I37" s="39" t="s">
         <v>33</v>
@@ -3391,11 +3394,11 @@
         <v>39</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" s="37"/>
       <c r="D38" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E38" s="38" t="s">
         <v>23</v>
@@ -3411,11 +3414,11 @@
         <v>39</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39" s="37"/>
       <c r="D39" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E39" s="38" t="s">
         <v>27</v>
@@ -3423,7 +3426,7 @@
       <c r="F39" s="38"/>
       <c r="G39" s="38"/>
       <c r="H39" s="40" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I39" s="38" t="s">
         <v>34</v>
@@ -3437,15 +3440,15 @@
         <v>39</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" s="37"/>
       <c r="D40" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E40" s="38"/>
       <c r="F40" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G40" s="38" t="s">
         <v>23</v>
@@ -3459,15 +3462,15 @@
         <v>39</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C41" s="37"/>
       <c r="D41" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E41" s="38"/>
       <c r="F41" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G41" s="38" t="s">
         <v>28</v>
@@ -3481,15 +3484,15 @@
         <v>39</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" s="37"/>
       <c r="D42" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E42" s="38"/>
       <c r="F42" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G42" s="38" t="s">
         <v>23</v>
@@ -3503,15 +3506,15 @@
         <v>39</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C43" s="37"/>
       <c r="D43" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E43" s="38"/>
       <c r="F43" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G43" s="38" t="s">
         <v>28</v>
@@ -3525,15 +3528,15 @@
         <v>39</v>
       </c>
       <c r="B44" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C44" s="37"/>
       <c r="D44" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E44" s="38"/>
       <c r="F44" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G44" s="38" t="s">
         <v>29</v>
@@ -3547,15 +3550,15 @@
         <v>39</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="37"/>
       <c r="D45" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E45" s="38"/>
       <c r="F45" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G45" s="38" t="s">
         <v>23</v>
@@ -3569,15 +3572,15 @@
         <v>39</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C46" s="37"/>
       <c r="D46" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E46" s="38"/>
       <c r="F46" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G46" s="38" t="s">
         <v>28</v>
@@ -3591,15 +3594,15 @@
         <v>39</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C47" s="37"/>
       <c r="D47" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E47" s="38"/>
       <c r="F47" s="38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G47" s="38" t="s">
         <v>23</v>
@@ -3613,15 +3616,15 @@
         <v>39</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48" s="37"/>
       <c r="D48" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E48" s="38"/>
       <c r="F48" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G48" s="38" t="s">
         <v>23</v>
@@ -3635,15 +3638,15 @@
         <v>39</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C49" s="37"/>
       <c r="D49" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E49" s="38"/>
       <c r="F49" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G49" s="38" t="s">
         <v>28</v>
@@ -3657,15 +3660,15 @@
         <v>39</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50" s="37"/>
       <c r="D50" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E50" s="38"/>
       <c r="F50" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G50" s="38" t="s">
         <v>23</v>
@@ -3679,15 +3682,15 @@
         <v>39</v>
       </c>
       <c r="B51" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C51" s="37"/>
       <c r="D51" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E51" s="38"/>
       <c r="F51" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G51" s="38" t="s">
         <v>28</v>
@@ -3701,15 +3704,15 @@
         <v>39</v>
       </c>
       <c r="B52" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C52" s="37"/>
       <c r="D52" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E52" s="38"/>
       <c r="F52" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G52" s="38" t="s">
         <v>23</v>
@@ -3723,15 +3726,15 @@
         <v>39</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C53" s="37"/>
       <c r="D53" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E53" s="38"/>
       <c r="F53" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G53" s="38" t="s">
         <v>23</v>
@@ -3745,15 +3748,15 @@
         <v>39</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E54" s="38"/>
       <c r="F54" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G54" s="38" t="s">
         <v>28</v>
@@ -3767,21 +3770,21 @@
         <v>39</v>
       </c>
       <c r="B55" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C55" s="37"/>
       <c r="D55" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E55" s="38"/>
       <c r="F55" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G55" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H55" s="39" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="I55" s="39" t="s">
         <v>33</v>
@@ -3795,21 +3798,21 @@
         <v>39</v>
       </c>
       <c r="B56" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C56" s="37"/>
       <c r="D56" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E56" s="38"/>
       <c r="F56" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G56" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H56" s="39" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="I56" s="39" t="s">
         <v>33</v>
@@ -3823,15 +3826,15 @@
         <v>39</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C57" s="37"/>
       <c r="D57" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E57" s="38"/>
       <c r="F57" s="38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G57" s="38" t="s">
         <v>23</v>
@@ -3845,15 +3848,15 @@
         <v>39</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E58" s="38"/>
       <c r="F58" s="38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G58" s="38" t="s">
         <v>28</v>
@@ -3867,15 +3870,15 @@
         <v>39</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C59" s="37"/>
       <c r="D59" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E59" s="38"/>
       <c r="F59" s="38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G59" s="38" t="s">
         <v>23</v>
@@ -3889,21 +3892,21 @@
         <v>39</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C60" s="37"/>
       <c r="D60" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E60" s="38"/>
       <c r="F60" s="38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G60" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H60" s="40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I60" s="39" t="s">
         <v>33</v>
@@ -3917,11 +3920,11 @@
         <v>39</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C61" s="37"/>
       <c r="D61" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E61" s="38" t="s">
         <v>23</v>
@@ -3937,15 +3940,15 @@
         <v>39</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C62" s="37"/>
       <c r="D62" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E62" s="38"/>
       <c r="F62" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G62" s="38" t="s">
         <v>23</v>
@@ -3959,15 +3962,15 @@
         <v>39</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E63" s="38"/>
       <c r="F63" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G63" s="38" t="s">
         <v>28</v>
@@ -3981,15 +3984,15 @@
         <v>39</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C64" s="37"/>
       <c r="D64" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E64" s="38"/>
       <c r="F64" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G64" s="38" t="s">
         <v>23</v>
@@ -4003,15 +4006,15 @@
         <v>39</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C65" s="37"/>
       <c r="D65" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E65" s="38"/>
       <c r="F65" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G65" s="38" t="s">
         <v>28</v>
@@ -4025,18 +4028,18 @@
         <v>39</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C66" s="37"/>
       <c r="D66" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E66" s="38"/>
       <c r="F66" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G66" s="38" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H66" s="40"/>
       <c r="I66" s="38"/>
@@ -4047,15 +4050,15 @@
         <v>39</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C67" s="37"/>
       <c r="D67" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E67" s="38"/>
       <c r="F67" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G67" s="38" t="s">
         <v>23</v>
@@ -4069,15 +4072,15 @@
         <v>39</v>
       </c>
       <c r="B68" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C68" s="37"/>
       <c r="D68" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E68" s="38"/>
       <c r="F68" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G68" s="38" t="s">
         <v>29</v>
@@ -4091,21 +4094,21 @@
         <v>39</v>
       </c>
       <c r="B69" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C69" s="37"/>
       <c r="D69" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E69" s="38"/>
       <c r="F69" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G69" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H69" s="40" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="I69" s="38" t="s">
         <v>33</v>
@@ -4119,15 +4122,15 @@
         <v>39</v>
       </c>
       <c r="B70" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C70" s="37"/>
       <c r="D70" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E70" s="38"/>
       <c r="F70" s="38" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G70" s="38" t="s">
         <v>23</v>
@@ -4141,15 +4144,15 @@
         <v>39</v>
       </c>
       <c r="B71" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C71" s="37"/>
       <c r="D71" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E71" s="38"/>
       <c r="F71" s="38" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G71" s="38" t="s">
         <v>28</v>
@@ -4163,15 +4166,15 @@
         <v>39</v>
       </c>
       <c r="B72" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C72" s="37"/>
       <c r="D72" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E72" s="38"/>
       <c r="F72" s="38" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G72" s="38" t="s">
         <v>24</v>
@@ -4185,15 +4188,15 @@
         <v>39</v>
       </c>
       <c r="B73" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C73" s="37"/>
       <c r="D73" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E73" s="38"/>
       <c r="F73" s="38" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G73" s="38" t="s">
         <v>23</v>
@@ -4207,15 +4210,15 @@
         <v>39</v>
       </c>
       <c r="B74" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C74" s="37"/>
       <c r="D74" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E74" s="38"/>
       <c r="F74" s="38" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G74" s="38" t="s">
         <v>28</v>
@@ -4229,15 +4232,15 @@
         <v>39</v>
       </c>
       <c r="B75" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C75" s="37"/>
       <c r="D75" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E75" s="38"/>
       <c r="F75" s="38" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G75" s="38" t="s">
         <v>23</v>
@@ -4251,15 +4254,15 @@
         <v>39</v>
       </c>
       <c r="B76" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C76" s="37"/>
       <c r="D76" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E76" s="38"/>
       <c r="F76" s="38" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G76" s="38" t="s">
         <v>23</v>
@@ -4273,15 +4276,15 @@
         <v>39</v>
       </c>
       <c r="B77" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C77" s="37"/>
       <c r="D77" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E77" s="38"/>
       <c r="F77" s="38" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G77" s="38" t="s">
         <v>24</v>
@@ -4295,21 +4298,21 @@
         <v>39</v>
       </c>
       <c r="B78" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C78" s="37"/>
       <c r="D78" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E78" s="38"/>
       <c r="F78" s="38" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G78" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H78" s="39" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I78" s="38" t="s">
         <v>33</v>
@@ -4323,7 +4326,7 @@
         <v>39</v>
       </c>
       <c r="B79" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C79" s="37"/>
       <c r="D79" s="38" t="s">
@@ -4343,7 +4346,7 @@
         <v>39</v>
       </c>
       <c r="B80" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C80" s="37"/>
       <c r="D80" s="38" t="s">
@@ -4355,7 +4358,7 @@
       <c r="F80" s="38"/>
       <c r="G80" s="38"/>
       <c r="H80" s="39" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I80" s="39" t="s">
         <v>33</v>
@@ -4369,7 +4372,7 @@
         <v>39</v>
       </c>
       <c r="B81" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C81" s="34" t="s">
         <v>23</v>
@@ -4387,7 +4390,7 @@
         <v>39</v>
       </c>
       <c r="B82" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C82" s="34" t="s">
         <v>29</v>
@@ -4405,7 +4408,7 @@
         <v>39</v>
       </c>
       <c r="B83" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C83" s="34" t="s">
         <v>23</v>
@@ -4423,11 +4426,11 @@
         <v>39</v>
       </c>
       <c r="B84" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C84" s="34"/>
       <c r="D84" s="41" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E84" s="41" t="s">
         <v>23</v>
@@ -4443,11 +4446,11 @@
         <v>39</v>
       </c>
       <c r="B85" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C85" s="34"/>
       <c r="D85" s="41" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E85" s="41" t="s">
         <v>28</v>
@@ -4463,11 +4466,11 @@
         <v>39</v>
       </c>
       <c r="B86" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C86" s="34"/>
       <c r="D86" s="41" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E86" s="41" t="s">
         <v>23</v>
@@ -4483,11 +4486,11 @@
         <v>39</v>
       </c>
       <c r="B87" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C87" s="34"/>
       <c r="D87" s="41" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E87" s="41" t="s">
         <v>28</v>
@@ -4503,11 +4506,11 @@
         <v>39</v>
       </c>
       <c r="B88" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C88" s="34"/>
       <c r="D88" s="41" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E88" s="41" t="s">
         <v>23</v>
@@ -4523,11 +4526,11 @@
         <v>39</v>
       </c>
       <c r="B89" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C89" s="34"/>
       <c r="D89" s="41" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E89" s="41" t="s">
         <v>23</v>
@@ -4543,7 +4546,7 @@
         <v>39</v>
       </c>
       <c r="B90" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C90" s="34"/>
       <c r="D90" s="41" t="s">
@@ -4563,7 +4566,7 @@
         <v>39</v>
       </c>
       <c r="B91" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C91" s="34"/>
       <c r="D91" s="41" t="s">
@@ -4575,7 +4578,7 @@
       <c r="F91" s="41"/>
       <c r="G91" s="41"/>
       <c r="H91" s="42" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I91" s="42" t="s">
         <v>33</v>
@@ -4589,7 +4592,7 @@
         <v>39</v>
       </c>
       <c r="B92" s="33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C92" s="43" t="s">
         <v>23</v>
@@ -4607,7 +4610,7 @@
         <v>39</v>
       </c>
       <c r="B93" s="33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C93" s="47" t="s">
         <v>28</v>
@@ -4625,7 +4628,7 @@
         <v>39</v>
       </c>
       <c r="B94" s="33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C94" s="46" t="s">
         <v>23</v>
@@ -4643,7 +4646,7 @@
         <v>39</v>
       </c>
       <c r="B95" s="33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C95" s="46"/>
       <c r="D95" s="44" t="s">
@@ -4663,7 +4666,7 @@
         <v>39</v>
       </c>
       <c r="B96" s="33" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C96" s="46"/>
       <c r="D96" s="44" t="s">
@@ -4675,7 +4678,7 @@
       <c r="F96" s="44"/>
       <c r="G96" s="44"/>
       <c r="H96" s="45" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I96" s="45" t="s">
         <v>33</v>
@@ -4717,7 +4720,7 @@
       <c r="F98" s="48"/>
       <c r="G98" s="48"/>
       <c r="H98" s="49" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I98" s="49" t="s">
         <v>34</v>
@@ -4741,7 +4744,7 @@
       <c r="F99" s="48"/>
       <c r="G99" s="48"/>
       <c r="H99" s="49" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I99" s="49" t="s">
         <v>33</v>
@@ -4755,7 +4758,7 @@
         <v>39</v>
       </c>
       <c r="B100" s="34" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C100" s="34" t="s">
         <v>22</v>
@@ -4777,10 +4780,10 @@
         <v>39</v>
       </c>
       <c r="B101" s="34" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C101" s="34" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D101" s="41"/>
       <c r="E101" s="41"/>

</xml_diff>

<commit_message>
guion 2 del grado 8. definitivos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/EsqueletoGuion_CS_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/EsqueletoGuion_CS_08_02_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -1758,7 +1758,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1768,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2561,7 +2561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D76" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+    <sheetView topLeftCell="D76" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
       <selection activeCell="H99" sqref="H99"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
guion 02 grados 8 y 9 ajustados
por revisar rec70 y rec170. Gracias
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/EsqueletoGuion_CS_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/EsqueletoGuion_CS_08_02_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="106">
   <si>
     <t>FICHA</t>
   </si>
@@ -199,9 +199,6 @@
     <t>La participación social</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: El sistema de castas</t>
-  </si>
-  <si>
     <t>Independencia de las colonias suramericanas</t>
   </si>
   <si>
@@ -347,6 +344,9 @@
   </si>
   <si>
     <t>La independencia de Centroamérica</t>
+  </si>
+  <si>
+    <t>El sistema de castas</t>
   </si>
 </sst>
 </file>
@@ -1758,7 +1758,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1768,7 +1768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1879,19 +1879,19 @@
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>88</v>
-      </c>
-      <c r="C2" t="s">
-        <v>89</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1907,19 +1907,19 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
         <v>87</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>88</v>
-      </c>
-      <c r="C3" t="s">
-        <v>89</v>
       </c>
       <c r="D3" t="s">
         <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1927,19 +1927,19 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
         <v>91</v>
-      </c>
-      <c r="B4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" t="s">
-        <v>92</v>
       </c>
       <c r="D4" t="s">
         <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -1947,19 +1947,19 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
         <v>91</v>
       </c>
-      <c r="B5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
         <v>92</v>
-      </c>
-      <c r="D5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" t="s">
-        <v>93</v>
       </c>
       <c r="F5">
         <v>9</v>
@@ -1967,19 +1967,19 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
         <v>91</v>
       </c>
-      <c r="B6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" t="s">
         <v>92</v>
-      </c>
-      <c r="D6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" t="s">
-        <v>93</v>
       </c>
       <c r="F6">
         <v>18</v>
@@ -2001,7 +2001,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2023,7 +2023,7 @@
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="54" t="s">
         <v>33</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="B6" s="54" t="s">
         <v>33</v>
@@ -2081,7 +2081,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="54" t="s">
         <v>33</v>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" s="54" t="s">
         <v>33</v>
@@ -2103,7 +2103,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="54" t="s">
         <v>33</v>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="54" t="s">
         <v>33</v>
@@ -2125,7 +2125,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" s="54" t="s">
         <v>33</v>
@@ -2136,7 +2136,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="54" t="s">
         <v>33</v>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="54" t="s">
         <v>33</v>
@@ -2158,7 +2158,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="54" t="s">
         <v>33</v>
@@ -2169,7 +2169,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" s="54" t="s">
         <v>33</v>
@@ -2235,7 +2235,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,7 +2273,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" s="51" t="s">
         <v>33</v>
@@ -2345,7 +2345,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="C9" s="51" t="s">
         <v>33</v>
@@ -2357,7 +2357,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="53" t="s">
         <v>34</v>
@@ -2369,7 +2369,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C11" s="51" t="s">
         <v>33</v>
@@ -2381,7 +2381,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="51" t="s">
         <v>33</v>
@@ -2393,7 +2393,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="51" t="s">
         <v>33</v>
@@ -2405,7 +2405,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="53" t="s">
         <v>34</v>
@@ -2417,7 +2417,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C15" s="51" t="s">
         <v>33</v>
@@ -2429,7 +2429,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C16" s="53" t="s">
         <v>34</v>
@@ -2441,7 +2441,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="51" t="s">
         <v>33</v>
@@ -2453,7 +2453,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="51" t="s">
         <v>33</v>
@@ -2465,7 +2465,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="53" t="s">
         <v>34</v>
@@ -2477,7 +2477,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C20" s="53" t="s">
         <v>33</v>
@@ -2559,10 +2559,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J112"/>
+  <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView topLeftCell="D76" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="H99" sqref="H99"/>
+    <sheetView tabSelected="1" topLeftCell="C73" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2614,7 +2614,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>23</v>
@@ -2632,7 +2632,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>28</v>
@@ -2650,7 +2650,7 @@
         <v>39</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>24</v>
@@ -2668,7 +2668,7 @@
         <v>39</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="20" t="s">
@@ -2688,7 +2688,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="20" t="s">
@@ -2708,7 +2708,7 @@
         <v>39</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="20" t="s">
@@ -2728,7 +2728,7 @@
         <v>39</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="20" t="s">
@@ -2754,7 +2754,7 @@
         <v>39</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="20" t="s">
@@ -2776,7 +2776,7 @@
         <v>39</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="20" t="s">
@@ -2790,7 +2790,7 @@
         <v>26</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I10" s="21" t="s">
         <v>33</v>
@@ -2804,7 +2804,7 @@
         <v>39</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="20" t="s">
@@ -2826,7 +2826,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="20" t="s">
@@ -2848,7 +2848,7 @@
         <v>39</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="20" t="s">
@@ -2870,7 +2870,7 @@
         <v>39</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="20" t="s">
@@ -2892,7 +2892,7 @@
         <v>39</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="20" t="s">
@@ -2914,7 +2914,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="20" t="s">
@@ -2936,7 +2936,7 @@
         <v>39</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="20" t="s">
@@ -2964,7 +2964,7 @@
         <v>39</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="20" t="s">
@@ -2992,7 +2992,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="22" t="s">
@@ -3012,7 +3012,7 @@
         <v>39</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="20" t="s">
@@ -3032,7 +3032,7 @@
         <v>39</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="20" t="s">
@@ -3052,7 +3052,7 @@
         <v>39</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22" s="23"/>
       <c r="D22" s="20" t="s">
@@ -3072,7 +3072,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="20" t="s">
@@ -3092,7 +3092,7 @@
         <v>39</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="20" t="s">
@@ -3118,7 +3118,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="20" t="s">
@@ -3138,7 +3138,7 @@
         <v>39</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26" s="23"/>
       <c r="D26" s="20" t="s">
@@ -3164,7 +3164,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27" s="23"/>
       <c r="D27" s="20" t="s">
@@ -3184,7 +3184,7 @@
         <v>39</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" s="20" t="s">
@@ -3204,7 +3204,7 @@
         <v>39</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C29" s="23"/>
       <c r="D29" s="20" t="s">
@@ -3224,7 +3224,7 @@
         <v>39</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="20" t="s">
@@ -3380,7 +3380,7 @@
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
       <c r="H37" s="39" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="I37" s="39" t="s">
         <v>33</v>
@@ -3398,7 +3398,7 @@
       </c>
       <c r="C38" s="37"/>
       <c r="D38" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E38" s="38" t="s">
         <v>23</v>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="C39" s="37"/>
       <c r="D39" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E39" s="38" t="s">
         <v>27</v>
@@ -3426,7 +3426,7 @@
       <c r="F39" s="38"/>
       <c r="G39" s="38"/>
       <c r="H39" s="40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I39" s="38" t="s">
         <v>34</v>
@@ -3444,11 +3444,11 @@
       </c>
       <c r="C40" s="37"/>
       <c r="D40" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E40" s="38"/>
       <c r="F40" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G40" s="38" t="s">
         <v>23</v>
@@ -3466,11 +3466,11 @@
       </c>
       <c r="C41" s="37"/>
       <c r="D41" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E41" s="38"/>
       <c r="F41" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G41" s="38" t="s">
         <v>28</v>
@@ -3488,11 +3488,11 @@
       </c>
       <c r="C42" s="37"/>
       <c r="D42" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E42" s="38"/>
       <c r="F42" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G42" s="38" t="s">
         <v>23</v>
@@ -3510,11 +3510,11 @@
       </c>
       <c r="C43" s="37"/>
       <c r="D43" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E43" s="38"/>
       <c r="F43" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G43" s="38" t="s">
         <v>28</v>
@@ -3532,11 +3532,11 @@
       </c>
       <c r="C44" s="37"/>
       <c r="D44" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E44" s="38"/>
       <c r="F44" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G44" s="38" t="s">
         <v>29</v>
@@ -3554,11 +3554,11 @@
       </c>
       <c r="C45" s="37"/>
       <c r="D45" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E45" s="38"/>
       <c r="F45" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G45" s="38" t="s">
         <v>23</v>
@@ -3576,11 +3576,11 @@
       </c>
       <c r="C46" s="37"/>
       <c r="D46" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E46" s="38"/>
       <c r="F46" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G46" s="38" t="s">
         <v>28</v>
@@ -3598,11 +3598,11 @@
       </c>
       <c r="C47" s="37"/>
       <c r="D47" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E47" s="38"/>
       <c r="F47" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G47" s="38" t="s">
         <v>23</v>
@@ -3620,11 +3620,11 @@
       </c>
       <c r="C48" s="37"/>
       <c r="D48" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E48" s="38"/>
       <c r="F48" s="38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G48" s="38" t="s">
         <v>23</v>
@@ -3642,11 +3642,11 @@
       </c>
       <c r="C49" s="37"/>
       <c r="D49" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E49" s="38"/>
       <c r="F49" s="38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G49" s="38" t="s">
         <v>28</v>
@@ -3664,11 +3664,11 @@
       </c>
       <c r="C50" s="37"/>
       <c r="D50" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E50" s="38"/>
       <c r="F50" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G50" s="38" t="s">
         <v>23</v>
@@ -3686,11 +3686,11 @@
       </c>
       <c r="C51" s="37"/>
       <c r="D51" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E51" s="38"/>
       <c r="F51" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G51" s="38" t="s">
         <v>28</v>
@@ -3708,11 +3708,11 @@
       </c>
       <c r="C52" s="37"/>
       <c r="D52" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E52" s="38"/>
       <c r="F52" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G52" s="38" t="s">
         <v>23</v>
@@ -3730,11 +3730,11 @@
       </c>
       <c r="C53" s="37"/>
       <c r="D53" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E53" s="38"/>
       <c r="F53" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G53" s="38" t="s">
         <v>23</v>
@@ -3752,11 +3752,11 @@
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E54" s="38"/>
       <c r="F54" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G54" s="38" t="s">
         <v>28</v>
@@ -3774,17 +3774,17 @@
       </c>
       <c r="C55" s="37"/>
       <c r="D55" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E55" s="38"/>
       <c r="F55" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G55" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H55" s="39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I55" s="39" t="s">
         <v>33</v>
@@ -3802,17 +3802,17 @@
       </c>
       <c r="C56" s="37"/>
       <c r="D56" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E56" s="38"/>
       <c r="F56" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G56" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H56" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I56" s="39" t="s">
         <v>33</v>
@@ -3830,11 +3830,11 @@
       </c>
       <c r="C57" s="37"/>
       <c r="D57" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E57" s="38"/>
       <c r="F57" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G57" s="38" t="s">
         <v>23</v>
@@ -3852,11 +3852,11 @@
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E58" s="38"/>
       <c r="F58" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G58" s="38" t="s">
         <v>28</v>
@@ -3874,11 +3874,11 @@
       </c>
       <c r="C59" s="37"/>
       <c r="D59" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E59" s="38"/>
       <c r="F59" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G59" s="38" t="s">
         <v>23</v>
@@ -3896,17 +3896,17 @@
       </c>
       <c r="C60" s="37"/>
       <c r="D60" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E60" s="38"/>
       <c r="F60" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G60" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H60" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I60" s="39" t="s">
         <v>33</v>
@@ -3924,7 +3924,7 @@
       </c>
       <c r="C61" s="37"/>
       <c r="D61" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E61" s="38" t="s">
         <v>23</v>
@@ -3944,11 +3944,11 @@
       </c>
       <c r="C62" s="37"/>
       <c r="D62" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E62" s="38"/>
       <c r="F62" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G62" s="38" t="s">
         <v>23</v>
@@ -3966,11 +3966,11 @@
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E63" s="38"/>
       <c r="F63" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G63" s="38" t="s">
         <v>28</v>
@@ -3988,11 +3988,11 @@
       </c>
       <c r="C64" s="37"/>
       <c r="D64" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E64" s="38"/>
       <c r="F64" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G64" s="38" t="s">
         <v>23</v>
@@ -4010,11 +4010,11 @@
       </c>
       <c r="C65" s="37"/>
       <c r="D65" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E65" s="38"/>
       <c r="F65" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G65" s="38" t="s">
         <v>28</v>
@@ -4032,11 +4032,11 @@
       </c>
       <c r="C66" s="37"/>
       <c r="D66" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E66" s="38"/>
       <c r="F66" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G66" s="38" t="s">
         <v>29</v>
@@ -4054,11 +4054,11 @@
       </c>
       <c r="C67" s="37"/>
       <c r="D67" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E67" s="38"/>
       <c r="F67" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G67" s="38" t="s">
         <v>23</v>
@@ -4076,11 +4076,11 @@
       </c>
       <c r="C68" s="37"/>
       <c r="D68" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E68" s="38"/>
       <c r="F68" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G68" s="38" t="s">
         <v>29</v>
@@ -4098,17 +4098,17 @@
       </c>
       <c r="C69" s="37"/>
       <c r="D69" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E69" s="38"/>
       <c r="F69" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G69" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H69" s="40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I69" s="38" t="s">
         <v>33</v>
@@ -4126,11 +4126,11 @@
       </c>
       <c r="C70" s="37"/>
       <c r="D70" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E70" s="38"/>
       <c r="F70" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G70" s="38" t="s">
         <v>23</v>
@@ -4148,11 +4148,11 @@
       </c>
       <c r="C71" s="37"/>
       <c r="D71" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E71" s="38"/>
       <c r="F71" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G71" s="38" t="s">
         <v>28</v>
@@ -4170,11 +4170,11 @@
       </c>
       <c r="C72" s="37"/>
       <c r="D72" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E72" s="38"/>
       <c r="F72" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G72" s="38" t="s">
         <v>24</v>
@@ -4192,11 +4192,11 @@
       </c>
       <c r="C73" s="37"/>
       <c r="D73" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E73" s="38"/>
       <c r="F73" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G73" s="38" t="s">
         <v>23</v>
@@ -4214,11 +4214,11 @@
       </c>
       <c r="C74" s="37"/>
       <c r="D74" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E74" s="38"/>
       <c r="F74" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G74" s="38" t="s">
         <v>28</v>
@@ -4236,11 +4236,11 @@
       </c>
       <c r="C75" s="37"/>
       <c r="D75" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E75" s="38"/>
       <c r="F75" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G75" s="38" t="s">
         <v>23</v>
@@ -4258,11 +4258,11 @@
       </c>
       <c r="C76" s="37"/>
       <c r="D76" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E76" s="38"/>
       <c r="F76" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G76" s="38" t="s">
         <v>23</v>
@@ -4280,11 +4280,11 @@
       </c>
       <c r="C77" s="37"/>
       <c r="D77" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E77" s="38"/>
       <c r="F77" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G77" s="38" t="s">
         <v>24</v>
@@ -4302,17 +4302,17 @@
       </c>
       <c r="C78" s="37"/>
       <c r="D78" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E78" s="38"/>
       <c r="F78" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G78" s="38" t="s">
         <v>26</v>
       </c>
       <c r="H78" s="39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I78" s="38" t="s">
         <v>33</v>
@@ -4322,23 +4322,17 @@
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B79" s="37" t="s">
-        <v>53</v>
-      </c>
+      <c r="A79" s="31"/>
+      <c r="B79" s="37"/>
       <c r="C79" s="37"/>
-      <c r="D79" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="E79" s="38" t="s">
-        <v>23</v>
-      </c>
+      <c r="D79" s="38"/>
+      <c r="E79" s="38"/>
       <c r="F79" s="38"/>
-      <c r="G79" s="38"/>
+      <c r="G79" s="38" t="s">
+        <v>28</v>
+      </c>
       <c r="H79" s="39"/>
-      <c r="I79" s="39"/>
+      <c r="I79" s="38"/>
       <c r="J79" s="27"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -4353,47 +4347,49 @@
         <v>25</v>
       </c>
       <c r="E80" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F80" s="38"/>
       <c r="G80" s="38"/>
-      <c r="H80" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="I80" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="J80" s="27">
-        <v>15</v>
-      </c>
+      <c r="H80" s="39"/>
+      <c r="I80" s="39"/>
+      <c r="J80" s="27"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B81" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C81" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="D81" s="41"/>
-      <c r="E81" s="41"/>
-      <c r="F81" s="41"/>
-      <c r="G81" s="41"/>
-      <c r="H81" s="42"/>
-      <c r="I81" s="42"/>
-      <c r="J81" s="27"/>
+      <c r="B81" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C81" s="37"/>
+      <c r="D81" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="E81" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F81" s="38"/>
+      <c r="G81" s="38"/>
+      <c r="H81" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="I81" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="J81" s="27">
+        <v>15</v>
+      </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="31" t="s">
         <v>39</v>
       </c>
       <c r="B82" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C82" s="34" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D82" s="41"/>
       <c r="E82" s="41"/>
@@ -4408,10 +4404,10 @@
         <v>39</v>
       </c>
       <c r="B83" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C83" s="34" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D83" s="41"/>
       <c r="E83" s="41"/>
@@ -4426,15 +4422,13 @@
         <v>39</v>
       </c>
       <c r="B84" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C84" s="34"/>
-      <c r="D84" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="E84" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="C84" s="34" t="s">
         <v>23</v>
       </c>
+      <c r="D84" s="41"/>
+      <c r="E84" s="41"/>
       <c r="F84" s="41"/>
       <c r="G84" s="41"/>
       <c r="H84" s="42"/>
@@ -4446,14 +4440,14 @@
         <v>39</v>
       </c>
       <c r="B85" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C85" s="34"/>
       <c r="D85" s="41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E85" s="41" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F85" s="41"/>
       <c r="G85" s="41"/>
@@ -4466,14 +4460,14 @@
         <v>39</v>
       </c>
       <c r="B86" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C86" s="34"/>
       <c r="D86" s="41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E86" s="41" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F86" s="41"/>
       <c r="G86" s="41"/>
@@ -4486,14 +4480,14 @@
         <v>39</v>
       </c>
       <c r="B87" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C87" s="34"/>
       <c r="D87" s="41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E87" s="41" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F87" s="41"/>
       <c r="G87" s="41"/>
@@ -4506,14 +4500,14 @@
         <v>39</v>
       </c>
       <c r="B88" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C88" s="34"/>
       <c r="D88" s="41" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E88" s="41" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F88" s="41"/>
       <c r="G88" s="41"/>
@@ -4526,11 +4520,11 @@
         <v>39</v>
       </c>
       <c r="B89" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C89" s="34"/>
       <c r="D89" s="41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E89" s="41" t="s">
         <v>23</v>
@@ -4546,11 +4540,11 @@
         <v>39</v>
       </c>
       <c r="B90" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C90" s="34"/>
       <c r="D90" s="41" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="E90" s="41" t="s">
         <v>23</v>
@@ -4566,54 +4560,56 @@
         <v>39</v>
       </c>
       <c r="B91" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C91" s="34"/>
       <c r="D91" s="41" t="s">
         <v>25</v>
       </c>
       <c r="E91" s="41" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F91" s="41"/>
       <c r="G91" s="41"/>
-      <c r="H91" s="42" t="s">
+      <c r="H91" s="42"/>
+      <c r="I91" s="42"/>
+      <c r="J91" s="27"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B92" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C92" s="34"/>
+      <c r="D92" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E92" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F92" s="41"/>
+      <c r="G92" s="41"/>
+      <c r="H92" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="I92" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="J92" s="27">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B93" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="I91" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="J91" s="27">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B92" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="C92" s="43" t="s">
+      <c r="C93" s="43" t="s">
         <v>23</v>
-      </c>
-      <c r="D92" s="44"/>
-      <c r="E92" s="44"/>
-      <c r="F92" s="44"/>
-      <c r="G92" s="44"/>
-      <c r="H92" s="45"/>
-      <c r="I92" s="45"/>
-      <c r="J92" s="27"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B93" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="C93" s="47" t="s">
-        <v>28</v>
       </c>
       <c r="D93" s="44"/>
       <c r="E93" s="44"/>
@@ -4628,10 +4624,10 @@
         <v>39</v>
       </c>
       <c r="B94" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="C94" s="46" t="s">
-        <v>23</v>
+        <v>78</v>
+      </c>
+      <c r="C94" s="47" t="s">
+        <v>28</v>
       </c>
       <c r="D94" s="44"/>
       <c r="E94" s="44"/>
@@ -4646,15 +4642,13 @@
         <v>39</v>
       </c>
       <c r="B95" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="C95" s="46"/>
-      <c r="D95" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="E95" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C95" s="46" t="s">
         <v>23</v>
       </c>
+      <c r="D95" s="44"/>
+      <c r="E95" s="44"/>
       <c r="F95" s="44"/>
       <c r="G95" s="44"/>
       <c r="H95" s="45"/>
@@ -4666,44 +4660,46 @@
         <v>39</v>
       </c>
       <c r="B96" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C96" s="46"/>
       <c r="D96" s="44" t="s">
         <v>25</v>
       </c>
       <c r="E96" s="44" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F96" s="44"/>
       <c r="G96" s="44"/>
-      <c r="H96" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="I96" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="J96" s="27">
-        <v>170</v>
-      </c>
+      <c r="H96" s="45"/>
+      <c r="I96" s="45"/>
+      <c r="J96" s="27"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B97" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C97" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="D97" s="48"/>
-      <c r="E97" s="48"/>
-      <c r="F97" s="48"/>
-      <c r="G97" s="48"/>
-      <c r="H97" s="49"/>
-      <c r="I97" s="49"/>
-      <c r="J97" s="27"/>
+      <c r="B97" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C97" s="46"/>
+      <c r="D97" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="E97" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="F97" s="44"/>
+      <c r="G97" s="44"/>
+      <c r="H97" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="I97" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="J97" s="27">
+        <v>170</v>
+      </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="31" t="s">
@@ -4713,21 +4709,15 @@
         <v>32</v>
       </c>
       <c r="C98" s="36" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D98" s="48"/>
       <c r="E98" s="48"/>
       <c r="F98" s="48"/>
       <c r="G98" s="48"/>
-      <c r="H98" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="I98" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="J98" s="27">
-        <v>180</v>
-      </c>
+      <c r="H98" s="49"/>
+      <c r="I98" s="49"/>
+      <c r="J98" s="27"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="31" t="s">
@@ -4744,35 +4734,37 @@
       <c r="F99" s="48"/>
       <c r="G99" s="48"/>
       <c r="H99" s="49" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I99" s="49" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J99" s="27">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B100" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="C100" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="D100" s="41"/>
-      <c r="E100" s="41"/>
-      <c r="F100" s="41"/>
-      <c r="G100" s="41"/>
-      <c r="H100" s="42"/>
-      <c r="I100" s="42" t="s">
+      <c r="B100" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C100" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D100" s="48"/>
+      <c r="E100" s="48"/>
+      <c r="F100" s="48"/>
+      <c r="G100" s="48"/>
+      <c r="H100" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="I100" s="49" t="s">
         <v>33</v>
       </c>
       <c r="J100" s="27">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
@@ -4780,44 +4772,66 @@
         <v>39</v>
       </c>
       <c r="B101" s="34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C101" s="34" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="D101" s="41"/>
       <c r="E101" s="41"/>
       <c r="F101" s="41"/>
       <c r="G101" s="41"/>
-      <c r="H101" s="42" t="s">
-        <v>21</v>
-      </c>
+      <c r="H101" s="42"/>
       <c r="I101" s="42" t="s">
         <v>33</v>
       </c>
       <c r="J101" s="27">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B102" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C102" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D102" s="41"/>
+      <c r="E102" s="41"/>
+      <c r="F102" s="41"/>
+      <c r="G102" s="41"/>
+      <c r="H102" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="I102" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="J102" s="27">
         <v>210</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>19</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="17" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B112" s="18" t="s">
+      <c r="B113" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C112" s="18" t="s">
+      <c r="C113" s="18" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Guion 2 Grado 8
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/EsqueletoGuion_CS_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/EsqueletoGuion_CS_08_02_CO.xlsx
@@ -1758,7 +1758,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2561,8 +2561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C73" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+    <sheetView tabSelected="1" topLeftCell="D70" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="H97" sqref="H97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>